<commit_message>
Added [DNA]; Updated physeq objects; fixed MiLineage to counts (not %)
</commit_message>
<xml_diff>
--- a/dna.xlsx
+++ b/dna.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/CRDS_Calcs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{9E0AF680-E717-4CAA-97FC-A56DA2999833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F660633C-ED1A-4904-B0C2-6EE7A653F313}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{9E0AF680-E717-4CAA-97FC-A56DA2999833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{083DB6AD-D1AE-44D8-A5CF-9D7649C4AA79}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dna" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="279">
   <si>
     <t>Sample</t>
   </si>
@@ -854,6 +854,9 @@
   </si>
   <si>
     <t>CT1_P41</t>
+  </si>
+  <si>
+    <t>CT1_S32</t>
   </si>
 </sst>
 </file>
@@ -1698,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5246,7 +5249,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>49</v>
+        <v>278</v>
       </c>
       <c r="B87" t="s">
         <v>13</v>

</xml_diff>